<commit_message>
Daily attendance processing - 2025-11-17 07:22:16
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Summary'!$A$1:$BF$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$494</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$502</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -43,7 +43,7 @@
       <color rgb="00000000"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill/>
     </fill>
@@ -137,7 +137,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFF1A6"/>
+        <fgColor rgb="003388D5"/>
       </patternFill>
     </fill>
     <fill>
@@ -148,6 +148,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00FF7C7C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF1A6"/>
       </patternFill>
     </fill>
     <fill>
@@ -171,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -243,7 +248,10 @@
     <xf numFmtId="0" fontId="1" fillId="21" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1008,11 +1016,11 @@
       </c>
       <c r="G2" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H2" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I2" s="13" t="n">
         <v>21</v>
@@ -1024,10 +1032,10 @@
         <v>29</v>
       </c>
       <c r="L2" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M2" s="13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N2" s="14" t="n">
         <v>5</v>
@@ -1076,7 +1084,7 @@
         <v>3</v>
       </c>
       <c r="Z2" s="16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="16" t="n">
         <v>0</v>
@@ -1231,16 +1239,16 @@
       </c>
       <c r="F3" s="22" t="inlineStr">
         <is>
-          <t>Low Risk</t>
+          <t>No Risk</t>
         </is>
       </c>
       <c r="G3" s="12" t="inlineStr">
         <is>
-          <t>20.7%</t>
+          <t>24.1%</t>
         </is>
       </c>
       <c r="H3" s="13" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="13" t="n">
         <v>21</v>
@@ -1252,10 +1260,10 @@
         <v>29</v>
       </c>
       <c r="L3" s="13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M3" s="13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3" s="14" t="n">
         <v>5</v>
@@ -1304,7 +1312,7 @@
         <v>3</v>
       </c>
       <c r="Z3" s="16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3" s="16" t="n">
         <v>0</v>
@@ -5561,7 +5569,7 @@
           <t>210935@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F22" s="22" t="inlineStr">
+      <c r="F22" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -10577,7 +10585,7 @@
           <t>211915@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F44" s="22" t="inlineStr">
+      <c r="F44" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -15137,7 +15145,7 @@
           <t>212322@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F64" s="22" t="inlineStr">
+      <c r="F64" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -15365,7 +15373,7 @@
           <t>212386@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F65" s="22" t="inlineStr">
+      <c r="F65" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -19697,18 +19705,18 @@
           <t>220766@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F84" s="11" t="inlineStr">
-        <is>
-          <t>Moderate Risk</t>
+      <c r="F84" s="25" t="inlineStr">
+        <is>
+          <t>Low Risk</t>
         </is>
       </c>
       <c r="G84" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H84" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I84" s="13" t="n">
         <v>21</v>
@@ -19720,10 +19728,10 @@
         <v>29</v>
       </c>
       <c r="L84" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M84" s="13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N84" s="14" t="n">
         <v>5</v>
@@ -19772,7 +19780,7 @@
         <v>3</v>
       </c>
       <c r="Z84" s="16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA84" s="16" t="n">
         <v>0</v>
@@ -20609,7 +20617,7 @@
           <t>220877@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F88" s="22" t="inlineStr">
+      <c r="F88" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -22889,7 +22897,7 @@
           <t>221022@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F98" s="22" t="inlineStr">
+      <c r="F98" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -26765,7 +26773,7 @@
           <t>221357@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F115" s="22" t="inlineStr">
+      <c r="F115" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -29273,18 +29281,18 @@
           <t>221435@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F126" s="11" t="inlineStr">
-        <is>
-          <t>Moderate Risk</t>
+      <c r="F126" s="25" t="inlineStr">
+        <is>
+          <t>Low Risk</t>
         </is>
       </c>
       <c r="G126" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H126" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I126" s="13" t="n">
         <v>21</v>
@@ -29296,10 +29304,10 @@
         <v>29</v>
       </c>
       <c r="L126" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M126" s="13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N126" s="14" t="n">
         <v>5</v>
@@ -29348,7 +29356,7 @@
         <v>3</v>
       </c>
       <c r="Z126" s="16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA126" s="16" t="n">
         <v>0</v>
@@ -30185,7 +30193,7 @@
           <t>221459@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F130" s="22" t="inlineStr">
+      <c r="F130" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -31097,18 +31105,18 @@
           <t>221494@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F134" s="22" t="inlineStr">
+      <c r="F134" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
       </c>
       <c r="G134" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H134" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I134" s="13" t="n">
         <v>21</v>
@@ -31120,10 +31128,10 @@
         <v>29</v>
       </c>
       <c r="L134" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M134" s="13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N134" s="14" t="n">
         <v>5</v>
@@ -31172,7 +31180,7 @@
         <v>3</v>
       </c>
       <c r="Z134" s="16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA134" s="16" t="n">
         <v>0</v>
@@ -33605,7 +33613,7 @@
           <t>221527@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F145" s="22" t="inlineStr">
+      <c r="F145" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -35885,7 +35893,7 @@
           <t>221579@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F155" s="22" t="inlineStr">
+      <c r="F155" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -37481,18 +37489,18 @@
           <t>221606@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F162" s="22" t="inlineStr">
+      <c r="F162" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
       </c>
       <c r="G162" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H162" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I162" s="13" t="n">
         <v>21</v>
@@ -37504,10 +37512,10 @@
         <v>29</v>
       </c>
       <c r="L162" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M162" s="13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N162" s="14" t="n">
         <v>5</v>
@@ -37556,7 +37564,7 @@
         <v>3</v>
       </c>
       <c r="Z162" s="16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA162" s="16" t="n">
         <v>0</v>
@@ -39768,11 +39776,11 @@
       </c>
       <c r="G172" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H172" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I172" s="13" t="n">
         <v>21</v>
@@ -39784,10 +39792,10 @@
         <v>29</v>
       </c>
       <c r="L172" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M172" s="13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N172" s="14" t="n">
         <v>5</v>
@@ -39836,7 +39844,7 @@
         <v>3</v>
       </c>
       <c r="Z172" s="16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA172" s="16" t="n">
         <v>0</v>
@@ -40673,7 +40681,7 @@
           <t>221682@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F176" s="22" t="inlineStr">
+      <c r="F176" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -42725,7 +42733,7 @@
           <t>221756@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F185" s="22" t="inlineStr">
+      <c r="F185" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -46145,7 +46153,7 @@
           <t>221850@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F200" s="22" t="inlineStr">
+      <c r="F200" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -49565,7 +49573,7 @@
           <t>221930@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F215" s="22" t="inlineStr">
+      <c r="F215" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -49793,18 +49801,18 @@
           <t>221933@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F216" s="24" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F216" s="11" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G216" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H216" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I216" s="13" t="n">
         <v>21</v>
@@ -49816,10 +49824,10 @@
         <v>29</v>
       </c>
       <c r="L216" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M216" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N216" s="14" t="n">
         <v>5</v>
@@ -49868,7 +49876,7 @@
         <v>3</v>
       </c>
       <c r="Z216" s="16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA216" s="16" t="n">
         <v>0</v>
@@ -50021,7 +50029,7 @@
           <t>221938@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F217" s="22" t="inlineStr">
+      <c r="F217" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -50477,7 +50485,7 @@
           <t>221944@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F219" s="22" t="inlineStr">
+      <c r="F219" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -53441,7 +53449,7 @@
           <t>222003@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F232" s="22" t="inlineStr">
+      <c r="F232" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -53669,7 +53677,7 @@
           <t>222004@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F233" s="22" t="inlineStr">
+      <c r="F233" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -54353,7 +54361,7 @@
           <t>222026@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F236" s="22" t="inlineStr">
+      <c r="F236" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -54809,7 +54817,7 @@
           <t>222028@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F238" s="22" t="inlineStr">
+      <c r="F238" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -55493,7 +55501,7 @@
           <t>222035@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F241" s="22" t="inlineStr">
+      <c r="F241" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -55949,7 +55957,7 @@
           <t>222053@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F243" s="22" t="inlineStr">
+      <c r="F243" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -56405,7 +56413,7 @@
           <t>222058@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F245" s="22" t="inlineStr">
+      <c r="F245" s="25" t="inlineStr">
         <is>
           <t>Low Risk</t>
         </is>
@@ -58215,7 +58223,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K494"/>
+  <dimension ref="A1:K502"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -58240,57 +58248,57 @@
   </cols>
   <sheetData>
     <row r="1" ht="22" customHeight="1">
-      <c r="A1" s="25" t="inlineStr">
+      <c r="A1" s="26" t="inlineStr">
         <is>
           <t>Student ID</t>
         </is>
       </c>
-      <c r="B1" s="25" t="inlineStr">
+      <c r="B1" s="26" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="25" t="inlineStr">
+      <c r="C1" s="26" t="inlineStr">
         <is>
           <t>Year</t>
         </is>
       </c>
-      <c r="D1" s="25" t="inlineStr">
+      <c r="D1" s="26" t="inlineStr">
         <is>
           <t>Group</t>
         </is>
       </c>
-      <c r="E1" s="25" t="inlineStr">
+      <c r="E1" s="26" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="F1" s="25" t="inlineStr">
+      <c r="F1" s="26" t="inlineStr">
         <is>
           <t>Subject</t>
         </is>
       </c>
-      <c r="G1" s="25" t="inlineStr">
+      <c r="G1" s="26" t="inlineStr">
         <is>
           <t>Session</t>
         </is>
       </c>
-      <c r="H1" s="25" t="inlineStr">
+      <c r="H1" s="26" t="inlineStr">
         <is>
           <t>Subject</t>
         </is>
       </c>
-      <c r="I1" s="25" t="inlineStr">
+      <c r="I1" s="26" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="J1" s="25" t="inlineStr">
+      <c r="J1" s="26" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="K1" s="25" t="inlineStr">
+      <c r="K1" s="26" t="inlineStr">
         <is>
           <t>Validation Group</t>
         </is>
@@ -62674,7 +62682,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J78" s="26" t="n">
+      <c r="J78" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K78" t="inlineStr">
@@ -62729,7 +62737,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J79" s="26" t="n">
+      <c r="J79" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K79" t="inlineStr">
@@ -62784,7 +62792,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J80" s="26" t="n">
+      <c r="J80" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K80" t="inlineStr">
@@ -62839,7 +62847,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J81" s="26" t="n">
+      <c r="J81" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K81" t="inlineStr">
@@ -62894,7 +62902,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J82" s="26" t="n">
+      <c r="J82" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K82" t="inlineStr">
@@ -62949,7 +62957,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J83" s="26" t="n">
+      <c r="J83" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K83" t="inlineStr">
@@ -63004,7 +63012,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J84" s="26" t="n">
+      <c r="J84" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K84" t="inlineStr">
@@ -63059,7 +63067,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J85" s="26" t="n">
+      <c r="J85" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K85" t="inlineStr">
@@ -63114,7 +63122,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J86" s="26" t="n">
+      <c r="J86" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K86" t="inlineStr">
@@ -63169,7 +63177,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J87" s="26" t="n">
+      <c r="J87" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K87" t="inlineStr">
@@ -63224,7 +63232,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J88" s="26" t="n">
+      <c r="J88" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K88" t="inlineStr">
@@ -63279,7 +63287,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J89" s="26" t="n">
+      <c r="J89" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K89" t="inlineStr">
@@ -63334,7 +63342,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J90" s="26" t="n">
+      <c r="J90" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K90" t="inlineStr">
@@ -63389,7 +63397,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J91" s="26" t="n">
+      <c r="J91" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K91" t="inlineStr">
@@ -63444,7 +63452,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J92" s="26" t="n">
+      <c r="J92" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K92" t="inlineStr">
@@ -63499,7 +63507,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J93" s="26" t="n">
+      <c r="J93" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K93" t="inlineStr">
@@ -63554,7 +63562,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J94" s="26" t="n">
+      <c r="J94" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K94" t="inlineStr">
@@ -63609,7 +63617,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J95" s="26" t="n">
+      <c r="J95" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K95" t="inlineStr">
@@ -63664,7 +63672,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J96" s="26" t="n">
+      <c r="J96" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K96" t="inlineStr">
@@ -63719,7 +63727,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J97" s="26" t="n">
+      <c r="J97" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K97" t="inlineStr">
@@ -63774,7 +63782,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J98" s="26" t="n">
+      <c r="J98" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K98" t="inlineStr">
@@ -63829,7 +63837,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J99" s="26" t="n">
+      <c r="J99" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K99" t="inlineStr">
@@ -63884,7 +63892,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J100" s="26" t="n">
+      <c r="J100" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K100" t="inlineStr">
@@ -63939,7 +63947,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J101" s="26" t="n">
+      <c r="J101" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K101" t="inlineStr">
@@ -63994,7 +64002,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J102" s="26" t="n">
+      <c r="J102" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K102" t="inlineStr">
@@ -64049,7 +64057,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J103" s="26" t="n">
+      <c r="J103" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K103" t="inlineStr">
@@ -64104,7 +64112,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J104" s="26" t="n">
+      <c r="J104" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K104" t="inlineStr">
@@ -64159,7 +64167,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J105" s="26" t="n">
+      <c r="J105" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K105" t="inlineStr">
@@ -64214,7 +64222,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J106" s="26" t="n">
+      <c r="J106" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K106" t="inlineStr">
@@ -64269,7 +64277,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J107" s="26" t="n">
+      <c r="J107" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K107" t="inlineStr">
@@ -64324,7 +64332,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J108" s="26" t="n">
+      <c r="J108" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K108" t="inlineStr">
@@ -64379,7 +64387,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J109" s="26" t="n">
+      <c r="J109" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K109" t="inlineStr">
@@ -64434,7 +64442,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J110" s="26" t="n">
+      <c r="J110" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K110" t="inlineStr">
@@ -64489,7 +64497,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J111" s="26" t="n">
+      <c r="J111" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K111" t="inlineStr">
@@ -64544,7 +64552,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J112" s="26" t="n">
+      <c r="J112" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K112" t="inlineStr">
@@ -64599,7 +64607,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J113" s="26" t="n">
+      <c r="J113" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K113" t="inlineStr">
@@ -64654,7 +64662,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J114" s="26" t="n">
+      <c r="J114" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K114" t="inlineStr">
@@ -64709,7 +64717,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J115" s="26" t="n">
+      <c r="J115" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K115" t="inlineStr">
@@ -64764,7 +64772,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J116" s="26" t="n">
+      <c r="J116" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K116" t="inlineStr">
@@ -64819,7 +64827,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J117" s="26" t="n">
+      <c r="J117" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K117" t="inlineStr">
@@ -64874,7 +64882,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J118" s="26" t="n">
+      <c r="J118" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K118" t="inlineStr">
@@ -64929,7 +64937,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J119" s="26" t="n">
+      <c r="J119" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K119" t="inlineStr">
@@ -64984,7 +64992,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J120" s="26" t="n">
+      <c r="J120" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K120" t="inlineStr">
@@ -65039,7 +65047,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J121" s="26" t="n">
+      <c r="J121" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K121" t="inlineStr">
@@ -65094,7 +65102,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J122" s="26" t="n">
+      <c r="J122" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K122" t="inlineStr">
@@ -65149,7 +65157,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J123" s="26" t="n">
+      <c r="J123" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K123" t="inlineStr">
@@ -65204,7 +65212,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J124" s="26" t="n">
+      <c r="J124" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K124" t="inlineStr">
@@ -65259,7 +65267,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J125" s="26" t="n">
+      <c r="J125" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K125" t="inlineStr">
@@ -65314,7 +65322,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J126" s="26" t="n">
+      <c r="J126" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K126" t="inlineStr">
@@ -65369,7 +65377,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J127" s="26" t="n">
+      <c r="J127" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K127" t="inlineStr">
@@ -65424,7 +65432,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J128" s="26" t="n">
+      <c r="J128" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K128" t="inlineStr">
@@ -65479,7 +65487,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J129" s="26" t="n">
+      <c r="J129" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K129" t="inlineStr">
@@ -65534,7 +65542,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J130" s="26" t="n">
+      <c r="J130" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K130" t="inlineStr">
@@ -65589,7 +65597,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J131" s="26" t="n">
+      <c r="J131" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K131" t="inlineStr">
@@ -65644,7 +65652,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J132" s="26" t="n">
+      <c r="J132" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K132" t="inlineStr">
@@ -65699,7 +65707,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J133" s="26" t="n">
+      <c r="J133" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K133" t="inlineStr">
@@ -65754,7 +65762,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J134" s="26" t="n">
+      <c r="J134" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K134" t="inlineStr">
@@ -65809,7 +65817,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J135" s="26" t="n">
+      <c r="J135" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K135" t="inlineStr">
@@ -65864,7 +65872,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J136" s="26" t="n">
+      <c r="J136" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K136" t="inlineStr">
@@ -65919,7 +65927,7 @@
           <t>29/10/2025</t>
         </is>
       </c>
-      <c r="J137" s="26" t="n">
+      <c r="J137" s="27" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="K137" t="inlineStr">
@@ -86277,8 +86285,464 @@
         </is>
       </c>
     </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>200540</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>محمد سعيد ابراهيم عواد درويش</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>200540@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F495" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="G495" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H495" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="I495" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J495" t="inlineStr">
+        <is>
+          <t>08:49:54</t>
+        </is>
+      </c>
+      <c r="K495" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>221606</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>راوية الطاهر عبدالله ناصر</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>221606@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F496" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="G496" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H496" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="I496" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J496" t="inlineStr">
+        <is>
+          <t>08:49:58</t>
+        </is>
+      </c>
+      <c r="K496" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>221654</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>محمد اسامه بابكر احمد</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E497" t="inlineStr">
+        <is>
+          <t>221654@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F497" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="G497" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H497" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="I497" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J497" t="inlineStr">
+        <is>
+          <t>08:50:01</t>
+        </is>
+      </c>
+      <c r="K497" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>221435</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>احمد سامى عثمان الدى</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E498" t="inlineStr">
+        <is>
+          <t>221435@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F498" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="G498" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H498" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="I498" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J498" t="inlineStr">
+        <is>
+          <t>08:50:04</t>
+        </is>
+      </c>
+      <c r="K498" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>221494</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>حسن الصادق مصطفى الحاج</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E499" t="inlineStr">
+        <is>
+          <t>221494@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F499" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="G499" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H499" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="I499" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J499" t="inlineStr">
+        <is>
+          <t>08:50:08</t>
+        </is>
+      </c>
+      <c r="K499" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>220766</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>ميار بنت خالد بن محمد الشيخ</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E500" t="inlineStr">
+        <is>
+          <t>220766@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F500" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="G500" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H500" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="I500" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J500" t="inlineStr">
+        <is>
+          <t>08:50:24</t>
+        </is>
+      </c>
+      <c r="K500" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>221933</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>معاذ انور عبدالله</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E501" t="inlineStr">
+        <is>
+          <t>221933@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F501" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="G501" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H501" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="I501" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J501" t="inlineStr">
+        <is>
+          <t>08:50:30</t>
+        </is>
+      </c>
+      <c r="K501" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>190252</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>عبد الله طلعت عبد اللطيف عواد شالق</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>190252@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F502" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="G502" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H502" t="inlineStr">
+        <is>
+          <t>HISTOLOGY</t>
+        </is>
+      </c>
+      <c r="I502" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J502" t="inlineStr">
+        <is>
+          <t>08:50:40</t>
+        </is>
+      </c>
+      <c r="K502" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K494"/>
+  <autoFilter ref="A1:K502"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Daily attendance processing - 2025-11-17 08:55:16
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Summary'!$A$1:$BF$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$502</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$518</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -19081,18 +19081,18 @@
           <t>220675@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F82" s="23" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F82" s="24" t="inlineStr">
+        <is>
+          <t>High Risk</t>
         </is>
       </c>
       <c r="G82" s="12" t="inlineStr">
         <is>
-          <t>3.4%</t>
+          <t>6.9%</t>
         </is>
       </c>
       <c r="H82" s="13" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I82" s="13" t="n">
         <v>20</v>
@@ -19104,16 +19104,16 @@
         <v>29</v>
       </c>
       <c r="L82" s="13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M82" s="13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N82" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O82" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P82" s="14" t="n">
         <v>0</v>
@@ -21574,11 +21574,11 @@
       </c>
       <c r="G93" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H93" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I93" s="13" t="n">
         <v>20</v>
@@ -21590,16 +21590,16 @@
         <v>29</v>
       </c>
       <c r="L93" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M93" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N93" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O93" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P93" s="14" t="n">
         <v>0</v>
@@ -22026,11 +22026,11 @@
       </c>
       <c r="G95" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H95" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I95" s="13" t="n">
         <v>20</v>
@@ -22042,16 +22042,16 @@
         <v>29</v>
       </c>
       <c r="L95" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="M95" s="13" t="n">
         <v>4</v>
-      </c>
-      <c r="M95" s="13" t="n">
-        <v>5</v>
       </c>
       <c r="N95" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O95" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P95" s="14" t="n">
         <v>1</v>
@@ -22252,11 +22252,11 @@
       </c>
       <c r="G96" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H96" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I96" s="13" t="n">
         <v>20</v>
@@ -22268,16 +22268,16 @@
         <v>29</v>
       </c>
       <c r="L96" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M96" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N96" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O96" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P96" s="14" t="n">
         <v>1</v>
@@ -24731,18 +24731,18 @@
           <t>221294@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F107" s="24" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F107" s="11" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G107" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H107" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I107" s="13" t="n">
         <v>20</v>
@@ -24754,16 +24754,16 @@
         <v>29</v>
       </c>
       <c r="L107" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M107" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N107" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O107" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P107" s="14" t="n">
         <v>0</v>
@@ -24957,18 +24957,18 @@
           <t>221307@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F108" s="24" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F108" s="11" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G108" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H108" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I108" s="13" t="n">
         <v>20</v>
@@ -24980,16 +24980,16 @@
         <v>29</v>
       </c>
       <c r="L108" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M108" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N108" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O108" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P108" s="14" t="n">
         <v>0</v>
@@ -25409,18 +25409,18 @@
           <t>221319@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F110" s="24" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F110" s="11" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G110" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H110" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I110" s="13" t="n">
         <v>20</v>
@@ -25432,16 +25432,16 @@
         <v>29</v>
       </c>
       <c r="L110" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M110" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N110" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O110" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P110" s="14" t="n">
         <v>1</v>
@@ -25635,18 +25635,18 @@
           <t>221324@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F111" s="24" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F111" s="11" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G111" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H111" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I111" s="13" t="n">
         <v>20</v>
@@ -25658,16 +25658,16 @@
         <v>29</v>
       </c>
       <c r="L111" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M111" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N111" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O111" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P111" s="14" t="n">
         <v>1</v>
@@ -26991,18 +26991,18 @@
           <t>221375@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F117" s="24" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F117" s="11" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G117" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H117" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I117" s="13" t="n">
         <v>20</v>
@@ -27014,16 +27014,16 @@
         <v>29</v>
       </c>
       <c r="L117" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M117" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N117" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O117" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P117" s="14" t="n">
         <v>0</v>
@@ -27224,11 +27224,11 @@
       </c>
       <c r="G118" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H118" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I118" s="13" t="n">
         <v>20</v>
@@ -27240,16 +27240,16 @@
         <v>29</v>
       </c>
       <c r="L118" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="M118" s="13" t="n">
         <v>4</v>
-      </c>
-      <c r="M118" s="13" t="n">
-        <v>5</v>
       </c>
       <c r="N118" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O118" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P118" s="14" t="n">
         <v>1</v>
@@ -27669,18 +27669,18 @@
           <t>221415@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F120" s="24" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F120" s="11" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G120" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H120" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I120" s="13" t="n">
         <v>20</v>
@@ -27692,16 +27692,16 @@
         <v>29</v>
       </c>
       <c r="L120" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M120" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N120" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O120" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P120" s="14" t="n">
         <v>0</v>
@@ -29025,18 +29025,18 @@
           <t>221435@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F126" s="11" t="inlineStr">
-        <is>
-          <t>Moderate Risk</t>
+      <c r="F126" s="22" t="inlineStr">
+        <is>
+          <t>Low Risk</t>
         </is>
       </c>
       <c r="G126" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H126" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I126" s="13" t="n">
         <v>20</v>
@@ -29048,16 +29048,16 @@
         <v>29</v>
       </c>
       <c r="L126" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M126" s="13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N126" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O126" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P126" s="14" t="n">
         <v>1</v>
@@ -29484,11 +29484,11 @@
       </c>
       <c r="G128" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H128" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I128" s="13" t="n">
         <v>20</v>
@@ -29500,16 +29500,16 @@
         <v>29</v>
       </c>
       <c r="L128" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M128" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N128" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O128" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P128" s="14" t="n">
         <v>0</v>
@@ -30162,11 +30162,11 @@
       </c>
       <c r="G131" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H131" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I131" s="13" t="n">
         <v>20</v>
@@ -30178,16 +30178,16 @@
         <v>29</v>
       </c>
       <c r="L131" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M131" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N131" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O131" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P131" s="14" t="n">
         <v>1</v>
@@ -30840,11 +30840,11 @@
       </c>
       <c r="G134" s="12" t="inlineStr">
         <is>
-          <t>20.7%</t>
+          <t>24.1%</t>
         </is>
       </c>
       <c r="H134" s="13" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I134" s="13" t="n">
         <v>20</v>
@@ -30856,16 +30856,16 @@
         <v>29</v>
       </c>
       <c r="L134" s="13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M134" s="13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N134" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O134" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P134" s="14" t="n">
         <v>1</v>
@@ -37620,11 +37620,11 @@
       </c>
       <c r="G164" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H164" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I164" s="13" t="n">
         <v>20</v>
@@ -37636,16 +37636,16 @@
         <v>29</v>
       </c>
       <c r="L164" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M164" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N164" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O164" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P164" s="14" t="n">
         <v>1</v>
@@ -57713,7 +57713,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K502"/>
+  <dimension ref="A1:K518"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -86231,8 +86231,920 @@
         </is>
       </c>
     </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>221435</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>احمد سامى عثمان الدى</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>221435@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F503" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G503" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H503" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I503" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J503" t="inlineStr">
+        <is>
+          <t>10:34:25</t>
+        </is>
+      </c>
+      <c r="K503" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>221494</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>حسن الصادق مصطفى الحاج</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E504" t="inlineStr">
+        <is>
+          <t>221494@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F504" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G504" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H504" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I504" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J504" t="inlineStr">
+        <is>
+          <t>10:34:30</t>
+        </is>
+      </c>
+      <c r="K504" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>220990</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>جاد زياد سلوم</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E505" t="inlineStr">
+        <is>
+          <t>220990@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F505" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G505" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H505" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I505" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J505" t="inlineStr">
+        <is>
+          <t>10:34:34</t>
+        </is>
+      </c>
+      <c r="K505" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>221438</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>كان فار نيانق كيج</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E506" t="inlineStr">
+        <is>
+          <t>221438@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F506" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G506" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H506" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I506" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J506" t="inlineStr">
+        <is>
+          <t>10:34:38</t>
+        </is>
+      </c>
+      <c r="K506" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>221415</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>داليا عبد العزيز مبروك عبد العزيز بكار</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E507" t="inlineStr">
+        <is>
+          <t>221415@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F507" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G507" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H507" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I507" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J507" t="inlineStr">
+        <is>
+          <t>10:34:43</t>
+        </is>
+      </c>
+      <c r="K507" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>221622</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>محمود محمد ادن</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E508" t="inlineStr">
+        <is>
+          <t>221622@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F508" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G508" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H508" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I508" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J508" t="inlineStr">
+        <is>
+          <t>10:34:50</t>
+        </is>
+      </c>
+      <c r="K508" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>221294</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>هاله يحى ابكر ابراهيم</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E509" t="inlineStr">
+        <is>
+          <t>221294@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F509" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G509" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H509" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I509" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J509" t="inlineStr">
+        <is>
+          <t>10:34:58</t>
+        </is>
+      </c>
+      <c r="K509" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>221375</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>محمد عمران محمد الهندى</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E510" t="inlineStr">
+        <is>
+          <t>221375@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F510" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G510" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H510" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I510" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J510" t="inlineStr">
+        <is>
+          <t>10:35:17</t>
+        </is>
+      </c>
+      <c r="K510" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>221404</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>محمد يزن محمد مازن ماوردى</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E511" t="inlineStr">
+        <is>
+          <t>221404@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F511" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G511" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H511" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I511" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J511" t="inlineStr">
+        <is>
+          <t>10:35:23</t>
+        </is>
+      </c>
+      <c r="K511" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>221324</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>مجد ذوقان خليل قيشاوي</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E512" t="inlineStr">
+        <is>
+          <t>221324@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F512" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G512" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H512" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I512" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J512" t="inlineStr">
+        <is>
+          <t>10:35:31</t>
+        </is>
+      </c>
+      <c r="K512" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>220675</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>محمد بدرالدين عبد العال عبد العال صبح</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E513" t="inlineStr">
+        <is>
+          <t>220675@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F513" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G513" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H513" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I513" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J513" t="inlineStr">
+        <is>
+          <t>10:35:36</t>
+        </is>
+      </c>
+      <c r="K513" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>221000</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>ابوبكر محمد قايد الثوابي</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E514" t="inlineStr">
+        <is>
+          <t>221000@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F514" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G514" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H514" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I514" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J514" t="inlineStr">
+        <is>
+          <t>10:35:55</t>
+        </is>
+      </c>
+      <c r="K514" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>221476</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>صالح هيثم صالح سواحلي</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E515" t="inlineStr">
+        <is>
+          <t>221476@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F515" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G515" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H515" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I515" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J515" t="inlineStr">
+        <is>
+          <t>10:36:02</t>
+        </is>
+      </c>
+      <c r="K515" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>220967</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>لارا حربي عبدالله الزيادات</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E516" t="inlineStr">
+        <is>
+          <t>220967@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F516" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G516" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H516" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I516" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J516" t="inlineStr">
+        <is>
+          <t>10:36:13</t>
+        </is>
+      </c>
+      <c r="K516" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>221319</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>روان صلاح طاهر الوهباني</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D517" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E517" t="inlineStr">
+        <is>
+          <t>221319@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F517" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G517" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H517" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I517" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J517" t="inlineStr">
+        <is>
+          <t>10:36:22</t>
+        </is>
+      </c>
+      <c r="K517" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>221307</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>دعاء عاصم على العوض</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D518" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E518" t="inlineStr">
+        <is>
+          <t>221307@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F518" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G518" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H518" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I518" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J518" t="inlineStr">
+        <is>
+          <t>10:36:29</t>
+        </is>
+      </c>
+      <c r="K518" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K502"/>
+  <autoFilter ref="A1:K518"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Daily attendance processing - 2025-11-17 15:23:48
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Summary'!$A$1:$BF$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$518</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$550</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -12208,11 +12208,11 @@
       </c>
       <c r="G52" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H52" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I52" s="13" t="n">
         <v>19</v>
@@ -12224,16 +12224,16 @@
         <v>29</v>
       </c>
       <c r="L52" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M52" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N52" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O52" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P52" s="14" t="n">
         <v>0</v>
@@ -12242,7 +12242,7 @@
         <v>1</v>
       </c>
       <c r="R52" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S52" s="14" t="inlineStr">
         <is>
@@ -15120,11 +15120,11 @@
       </c>
       <c r="G65" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H65" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I65" s="13" t="n">
         <v>19</v>
@@ -15136,16 +15136,16 @@
         <v>29</v>
       </c>
       <c r="L65" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M65" s="13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N65" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O65" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P65" s="14" t="n">
         <v>1</v>
@@ -15154,7 +15154,7 @@
         <v>1</v>
       </c>
       <c r="R65" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S65" s="14" t="inlineStr">
         <is>
@@ -25648,11 +25648,11 @@
       </c>
       <c r="G112" s="12" t="inlineStr">
         <is>
-          <t>3.4%</t>
+          <t>6.9%</t>
         </is>
       </c>
       <c r="H112" s="13" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I112" s="13" t="n">
         <v>19</v>
@@ -25664,16 +25664,16 @@
         <v>29</v>
       </c>
       <c r="L112" s="13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M112" s="13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N112" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O112" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P112" s="14" t="n">
         <v>0</v>
@@ -25682,7 +25682,7 @@
         <v>1</v>
       </c>
       <c r="R112" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S112" s="14" t="inlineStr">
         <is>
@@ -26320,11 +26320,11 @@
       </c>
       <c r="G115" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H115" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I115" s="13" t="n">
         <v>19</v>
@@ -26336,16 +26336,16 @@
         <v>29</v>
       </c>
       <c r="L115" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M115" s="13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N115" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O115" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P115" s="14" t="n">
         <v>1</v>
@@ -26354,7 +26354,7 @@
         <v>1</v>
       </c>
       <c r="R115" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S115" s="14" t="inlineStr">
         <is>
@@ -29680,11 +29680,11 @@
       </c>
       <c r="G130" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H130" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I130" s="13" t="n">
         <v>19</v>
@@ -29696,16 +29696,16 @@
         <v>29</v>
       </c>
       <c r="L130" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M130" s="13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N130" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O130" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P130" s="14" t="n">
         <v>1</v>
@@ -29714,7 +29714,7 @@
         <v>1</v>
       </c>
       <c r="R130" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S130" s="14" t="inlineStr">
         <is>
@@ -33257,18 +33257,18 @@
           <t>221536@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F146" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F146" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G146" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H146" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I146" s="13" t="n">
         <v>19</v>
@@ -33280,16 +33280,16 @@
         <v>29</v>
       </c>
       <c r="L146" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M146" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N146" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O146" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P146" s="14" t="n">
         <v>0</v>
@@ -33298,7 +33298,7 @@
         <v>0</v>
       </c>
       <c r="R146" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S146" s="14" t="inlineStr">
         <is>
@@ -33481,18 +33481,18 @@
           <t>221539@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F147" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F147" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G147" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H147" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I147" s="13" t="n">
         <v>19</v>
@@ -33504,16 +33504,16 @@
         <v>29</v>
       </c>
       <c r="L147" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M147" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N147" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O147" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P147" s="14" t="n">
         <v>0</v>
@@ -33522,7 +33522,7 @@
         <v>1</v>
       </c>
       <c r="R147" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S147" s="14" t="inlineStr">
         <is>
@@ -34160,11 +34160,11 @@
       </c>
       <c r="G150" s="12" t="inlineStr">
         <is>
-          <t>3.4%</t>
+          <t>6.9%</t>
         </is>
       </c>
       <c r="H150" s="13" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I150" s="13" t="n">
         <v>19</v>
@@ -34176,16 +34176,16 @@
         <v>29</v>
       </c>
       <c r="L150" s="13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M150" s="13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N150" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O150" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P150" s="14" t="n">
         <v>0</v>
@@ -34194,7 +34194,7 @@
         <v>0</v>
       </c>
       <c r="R150" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S150" s="14" t="inlineStr">
         <is>
@@ -34608,11 +34608,11 @@
       </c>
       <c r="G152" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H152" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I152" s="13" t="n">
         <v>19</v>
@@ -34624,16 +34624,16 @@
         <v>29</v>
       </c>
       <c r="L152" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M152" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N152" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O152" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P152" s="14" t="n">
         <v>1</v>
@@ -34642,7 +34642,7 @@
         <v>0</v>
       </c>
       <c r="R152" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S152" s="14" t="inlineStr">
         <is>
@@ -35280,11 +35280,11 @@
       </c>
       <c r="G155" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H155" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I155" s="13" t="n">
         <v>19</v>
@@ -35296,16 +35296,16 @@
         <v>29</v>
       </c>
       <c r="L155" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M155" s="13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N155" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O155" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P155" s="14" t="n">
         <v>1</v>
@@ -35314,7 +35314,7 @@
         <v>1</v>
       </c>
       <c r="R155" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S155" s="14" t="inlineStr">
         <is>
@@ -36169,18 +36169,18 @@
           <t>221589@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F159" s="23" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F159" s="11" t="inlineStr">
+        <is>
+          <t>High Risk</t>
         </is>
       </c>
       <c r="G159" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H159" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I159" s="13" t="n">
         <v>19</v>
@@ -36192,16 +36192,16 @@
         <v>29</v>
       </c>
       <c r="L159" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M159" s="13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N159" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O159" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P159" s="14" t="n">
         <v>0</v>
@@ -36210,7 +36210,7 @@
         <v>0</v>
       </c>
       <c r="R159" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S159" s="14" t="inlineStr">
         <is>
@@ -36393,18 +36393,18 @@
           <t>221599@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F160" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F160" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G160" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H160" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I160" s="13" t="n">
         <v>19</v>
@@ -36416,16 +36416,16 @@
         <v>29</v>
       </c>
       <c r="L160" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M160" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N160" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O160" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P160" s="14" t="n">
         <v>1</v>
@@ -36434,7 +36434,7 @@
         <v>1</v>
       </c>
       <c r="R160" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S160" s="14" t="inlineStr">
         <is>
@@ -36617,18 +36617,18 @@
           <t>221600@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F161" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F161" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G161" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H161" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I161" s="13" t="n">
         <v>19</v>
@@ -36640,16 +36640,16 @@
         <v>29</v>
       </c>
       <c r="L161" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M161" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N161" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O161" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P161" s="14" t="n">
         <v>1</v>
@@ -36658,7 +36658,7 @@
         <v>1</v>
       </c>
       <c r="R161" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S161" s="14" t="inlineStr">
         <is>
@@ -36841,18 +36841,18 @@
           <t>221606@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F162" s="24" t="inlineStr">
-        <is>
-          <t>Moderate Risk</t>
+      <c r="F162" s="22" t="inlineStr">
+        <is>
+          <t>Low Risk</t>
         </is>
       </c>
       <c r="G162" s="12" t="inlineStr">
         <is>
-          <t>20.7%</t>
+          <t>24.1%</t>
         </is>
       </c>
       <c r="H162" s="13" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I162" s="13" t="n">
         <v>19</v>
@@ -36864,16 +36864,16 @@
         <v>29</v>
       </c>
       <c r="L162" s="13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M162" s="13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N162" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O162" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P162" s="14" t="n">
         <v>1</v>
@@ -36882,7 +36882,7 @@
         <v>1</v>
       </c>
       <c r="R162" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S162" s="14" t="inlineStr">
         <is>
@@ -37744,11 +37744,11 @@
       </c>
       <c r="G166" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H166" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I166" s="13" t="n">
         <v>19</v>
@@ -37760,16 +37760,16 @@
         <v>29</v>
       </c>
       <c r="L166" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M166" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N166" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O166" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P166" s="14" t="n">
         <v>1</v>
@@ -37778,7 +37778,7 @@
         <v>0</v>
       </c>
       <c r="R166" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S166" s="14" t="inlineStr">
         <is>
@@ -38857,18 +38857,18 @@
           <t>221653@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F171" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F171" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G171" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H171" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I171" s="13" t="n">
         <v>19</v>
@@ -38880,16 +38880,16 @@
         <v>29</v>
       </c>
       <c r="L171" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M171" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N171" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O171" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P171" s="14" t="n">
         <v>0</v>
@@ -38898,7 +38898,7 @@
         <v>1</v>
       </c>
       <c r="R171" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S171" s="14" t="inlineStr">
         <is>
@@ -39081,18 +39081,18 @@
           <t>221654@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F172" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F172" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G172" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H172" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I172" s="13" t="n">
         <v>19</v>
@@ -39104,16 +39104,16 @@
         <v>29</v>
       </c>
       <c r="L172" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M172" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N172" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O172" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P172" s="14" t="n">
         <v>0</v>
@@ -39122,7 +39122,7 @@
         <v>1</v>
       </c>
       <c r="R172" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S172" s="14" t="inlineStr">
         <is>
@@ -39529,18 +39529,18 @@
           <t>221668@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F174" s="23" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F174" s="11" t="inlineStr">
+        <is>
+          <t>High Risk</t>
         </is>
       </c>
       <c r="G174" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H174" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I174" s="13" t="n">
         <v>19</v>
@@ -39552,16 +39552,16 @@
         <v>29</v>
       </c>
       <c r="L174" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M174" s="13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N174" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O174" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P174" s="14" t="n">
         <v>0</v>
@@ -39570,7 +39570,7 @@
         <v>0</v>
       </c>
       <c r="R174" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S174" s="14" t="inlineStr">
         <is>
@@ -39753,18 +39753,18 @@
           <t>221675@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F175" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F175" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G175" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H175" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I175" s="13" t="n">
         <v>19</v>
@@ -39776,16 +39776,16 @@
         <v>29</v>
       </c>
       <c r="L175" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M175" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N175" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O175" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P175" s="14" t="n">
         <v>1</v>
@@ -39794,7 +39794,7 @@
         <v>1</v>
       </c>
       <c r="R175" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S175" s="14" t="inlineStr">
         <is>
@@ -41769,18 +41769,18 @@
           <t>221755@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F184" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F184" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G184" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H184" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I184" s="13" t="n">
         <v>19</v>
@@ -41792,16 +41792,16 @@
         <v>29</v>
       </c>
       <c r="L184" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M184" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N184" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O184" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P184" s="14" t="n">
         <v>0</v>
@@ -41810,7 +41810,7 @@
         <v>1</v>
       </c>
       <c r="R184" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S184" s="14" t="inlineStr">
         <is>
@@ -42000,11 +42000,11 @@
       </c>
       <c r="G185" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H185" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I185" s="13" t="n">
         <v>19</v>
@@ -42016,16 +42016,16 @@
         <v>29</v>
       </c>
       <c r="L185" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M185" s="13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N185" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O185" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P185" s="14" t="n">
         <v>1</v>
@@ -42034,7 +42034,7 @@
         <v>1</v>
       </c>
       <c r="R185" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S185" s="14" t="inlineStr">
         <is>
@@ -42672,11 +42672,11 @@
       </c>
       <c r="G188" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H188" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I188" s="13" t="n">
         <v>19</v>
@@ -42688,16 +42688,16 @@
         <v>29</v>
       </c>
       <c r="L188" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M188" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N188" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O188" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P188" s="14" t="n">
         <v>0</v>
@@ -42706,7 +42706,7 @@
         <v>1</v>
       </c>
       <c r="R188" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S188" s="14" t="inlineStr">
         <is>
@@ -44240,11 +44240,11 @@
       </c>
       <c r="G195" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H195" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I195" s="13" t="n">
         <v>19</v>
@@ -44256,16 +44256,16 @@
         <v>29</v>
       </c>
       <c r="L195" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M195" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N195" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O195" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P195" s="14" t="n">
         <v>0</v>
@@ -44274,7 +44274,7 @@
         <v>1</v>
       </c>
       <c r="R195" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S195" s="14" t="inlineStr">
         <is>
@@ -44457,18 +44457,18 @@
           <t>221826@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F196" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F196" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G196" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H196" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I196" s="13" t="n">
         <v>19</v>
@@ -44480,16 +44480,16 @@
         <v>29</v>
       </c>
       <c r="L196" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M196" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N196" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O196" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P196" s="14" t="n">
         <v>0</v>
@@ -44498,7 +44498,7 @@
         <v>1</v>
       </c>
       <c r="R196" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S196" s="14" t="inlineStr">
         <is>
@@ -46025,18 +46025,18 @@
           <t>221866@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F203" s="23" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F203" s="11" t="inlineStr">
+        <is>
+          <t>High Risk</t>
         </is>
       </c>
       <c r="G203" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H203" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I203" s="13" t="n">
         <v>19</v>
@@ -46048,16 +46048,16 @@
         <v>29</v>
       </c>
       <c r="L203" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M203" s="13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N203" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O203" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P203" s="14" t="n">
         <v>0</v>
@@ -46066,7 +46066,7 @@
         <v>1</v>
       </c>
       <c r="R203" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S203" s="14" t="inlineStr">
         <is>
@@ -46928,11 +46928,11 @@
       </c>
       <c r="G207" s="12" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>3.4%</t>
         </is>
       </c>
       <c r="H207" s="13" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I207" s="13" t="n">
         <v>19</v>
@@ -46944,16 +46944,16 @@
         <v>29</v>
       </c>
       <c r="L207" s="13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M207" s="13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N207" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O207" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P207" s="14" t="n">
         <v>0</v>
@@ -46962,7 +46962,7 @@
         <v>0</v>
       </c>
       <c r="R207" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S207" s="14" t="inlineStr">
         <is>
@@ -47369,18 +47369,18 @@
           <t>221904@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F209" s="23" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F209" s="11" t="inlineStr">
+        <is>
+          <t>High Risk</t>
         </is>
       </c>
       <c r="G209" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H209" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I209" s="13" t="n">
         <v>19</v>
@@ -47392,16 +47392,16 @@
         <v>29</v>
       </c>
       <c r="L209" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M209" s="13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N209" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O209" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P209" s="14" t="n">
         <v>0</v>
@@ -47410,7 +47410,7 @@
         <v>1</v>
       </c>
       <c r="R209" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S209" s="14" t="inlineStr">
         <is>
@@ -47600,11 +47600,11 @@
       </c>
       <c r="G210" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H210" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I210" s="13" t="n">
         <v>19</v>
@@ -47616,16 +47616,16 @@
         <v>29</v>
       </c>
       <c r="L210" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M210" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N210" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O210" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P210" s="14" t="n">
         <v>0</v>
@@ -47634,7 +47634,7 @@
         <v>1</v>
       </c>
       <c r="R210" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S210" s="14" t="inlineStr">
         <is>
@@ -48048,11 +48048,11 @@
       </c>
       <c r="G212" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H212" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I212" s="13" t="n">
         <v>19</v>
@@ -48064,16 +48064,16 @@
         <v>29</v>
       </c>
       <c r="L212" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M212" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N212" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O212" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P212" s="14" t="n">
         <v>0</v>
@@ -48082,7 +48082,7 @@
         <v>1</v>
       </c>
       <c r="R212" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S212" s="14" t="inlineStr">
         <is>
@@ -48944,11 +48944,11 @@
       </c>
       <c r="G216" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H216" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I216" s="13" t="n">
         <v>19</v>
@@ -48960,16 +48960,16 @@
         <v>29</v>
       </c>
       <c r="L216" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M216" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N216" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O216" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P216" s="14" t="n">
         <v>0</v>
@@ -48978,7 +48978,7 @@
         <v>1</v>
       </c>
       <c r="R216" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S216" s="14" t="inlineStr">
         <is>
@@ -50953,18 +50953,18 @@
           <t>221966@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F225" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F225" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G225" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H225" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I225" s="13" t="n">
         <v>19</v>
@@ -50976,16 +50976,16 @@
         <v>29</v>
       </c>
       <c r="L225" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M225" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N225" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O225" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P225" s="14" t="n">
         <v>0</v>
@@ -50994,7 +50994,7 @@
         <v>1</v>
       </c>
       <c r="R225" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S225" s="14" t="inlineStr">
         <is>
@@ -52745,18 +52745,18 @@
           <t>222004@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F233" s="24" t="inlineStr">
-        <is>
-          <t>Moderate Risk</t>
+      <c r="F233" s="22" t="inlineStr">
+        <is>
+          <t>Low Risk</t>
         </is>
       </c>
       <c r="G233" s="12" t="inlineStr">
         <is>
-          <t>20.7%</t>
+          <t>24.1%</t>
         </is>
       </c>
       <c r="H233" s="13" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I233" s="13" t="n">
         <v>19</v>
@@ -52768,16 +52768,16 @@
         <v>29</v>
       </c>
       <c r="L233" s="13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M233" s="13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N233" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O233" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P233" s="14" t="n">
         <v>1</v>
@@ -52786,7 +52786,7 @@
         <v>1</v>
       </c>
       <c r="R233" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S233" s="14" t="inlineStr">
         <is>
@@ -57211,7 +57211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K518"/>
+  <dimension ref="A1:K550"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -86641,8 +86641,1832 @@
         </is>
       </c>
     </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>221822</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>سعادة يوسف عليو</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E519" t="inlineStr">
+        <is>
+          <t>221822@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F519" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G519" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H519" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I519" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J519" t="inlineStr">
+        <is>
+          <t>10:38:30</t>
+        </is>
+      </c>
+      <c r="K519" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>221826</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>بخيتة اوت قور كول</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D520" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E520" t="inlineStr">
+        <is>
+          <t>221826@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F520" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G520" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H520" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I520" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J520" t="inlineStr">
+        <is>
+          <t>10:38:40</t>
+        </is>
+      </c>
+      <c r="K520" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>212386</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>لويد اليكس موجا</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D521" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E521" t="inlineStr">
+        <is>
+          <t>212386@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F521" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G521" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H521" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I521" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J521" t="inlineStr">
+        <is>
+          <t>10:39:02</t>
+        </is>
+      </c>
+      <c r="K521" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>221755</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>سعدية عاشق</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E522" t="inlineStr">
+        <is>
+          <t>221755@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F522" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G522" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H522" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I522" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J522" t="inlineStr">
+        <is>
+          <t>10:39:08</t>
+        </is>
+      </c>
+      <c r="K522" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>221539</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>تحريم شوكات مالك</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E523" t="inlineStr">
+        <is>
+          <t>221539@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F523" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G523" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H523" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I523" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J523" t="inlineStr">
+        <is>
+          <t>10:39:13</t>
+        </is>
+      </c>
+      <c r="K523" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>221866</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>امينة موسى رمبو</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E524" t="inlineStr">
+        <is>
+          <t>221866@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F524" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G524" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H524" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I524" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J524" t="inlineStr">
+        <is>
+          <t>10:39:17</t>
+        </is>
+      </c>
+      <c r="K524" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>221914</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>معز اشتياق</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E525" t="inlineStr">
+        <is>
+          <t>221914@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F525" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G525" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H525" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I525" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J525" t="inlineStr">
+        <is>
+          <t>10:39:28</t>
+        </is>
+      </c>
+      <c r="K525" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>212145</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>سميه لاوان شايبو</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E526" t="inlineStr">
+        <is>
+          <t>212145@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F526" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G526" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H526" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I526" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J526" t="inlineStr">
+        <is>
+          <t>10:39:39</t>
+        </is>
+      </c>
+      <c r="K526" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>221329</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>خديجة اولو اتوين ادونبكو</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E527" t="inlineStr">
+        <is>
+          <t>221329@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F527" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G527" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H527" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I527" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J527" t="inlineStr">
+        <is>
+          <t>10:40:02</t>
+        </is>
+      </c>
+      <c r="K527" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>221895</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>عمر ادول فاروق</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D528" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E528" t="inlineStr">
+        <is>
+          <t>221895@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F528" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G528" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H528" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I528" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J528" t="inlineStr">
+        <is>
+          <t>10:40:13</t>
+        </is>
+      </c>
+      <c r="K528" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>221966</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>ساكى جوزيف اليساما زونقبيتى</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D529" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E529" t="inlineStr">
+        <is>
+          <t>221966@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F529" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G529" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H529" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I529" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J529" t="inlineStr">
+        <is>
+          <t>10:20:23</t>
+        </is>
+      </c>
+      <c r="K529" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>221599</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>سلمى عبد الرحمن عبيد موسى</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D530" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E530" t="inlineStr">
+        <is>
+          <t>221599@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F530" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G530" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H530" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I530" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J530" t="inlineStr">
+        <is>
+          <t>10:20:26</t>
+        </is>
+      </c>
+      <c r="K530" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>221909</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>ديكتور يمبيك بول نيان</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D531" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E531" t="inlineStr">
+        <is>
+          <t>221909@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F531" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G531" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H531" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I531" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J531" t="inlineStr">
+        <is>
+          <t>10:20:30</t>
+        </is>
+      </c>
+      <c r="K531" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>221904</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>عائشه نور شيهو</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D532" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E532" t="inlineStr">
+        <is>
+          <t>221904@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F532" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G532" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H532" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I532" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J532" t="inlineStr">
+        <is>
+          <t>10:20:33</t>
+        </is>
+      </c>
+      <c r="K532" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>221774</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>يدجوك جيمس كوانقو اكوك</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D533" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E533" t="inlineStr">
+        <is>
+          <t>221774@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F533" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G533" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H533" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I533" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J533" t="inlineStr">
+        <is>
+          <t>10:20:37</t>
+        </is>
+      </c>
+      <c r="K533" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>221933</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>معاذ انور عبدالله</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D534" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E534" t="inlineStr">
+        <is>
+          <t>221933@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F534" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G534" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H534" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I534" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J534" t="inlineStr">
+        <is>
+          <t>10:20:41</t>
+        </is>
+      </c>
+      <c r="K534" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>221668</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>محمد اسامه حسين</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D535" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E535" t="inlineStr">
+        <is>
+          <t>221668@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F535" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G535" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H535" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I535" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J535" t="inlineStr">
+        <is>
+          <t>10:20:44</t>
+        </is>
+      </c>
+      <c r="K535" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>221600</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>مروان معاوية عثمان الطيب</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D536" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E536" t="inlineStr">
+        <is>
+          <t>221600@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F536" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G536" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H536" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I536" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J536" t="inlineStr">
+        <is>
+          <t>10:16:50</t>
+        </is>
+      </c>
+      <c r="K536" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>221558</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>محمد عادل عوض باحاج</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D537" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E537" t="inlineStr">
+        <is>
+          <t>221558@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F537" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G537" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H537" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I537" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J537" t="inlineStr">
+        <is>
+          <t>10:16:55</t>
+        </is>
+      </c>
+      <c r="K537" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>222004</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>احمد ايمن احمد بشير</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D538" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E538" t="inlineStr">
+        <is>
+          <t>222004@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F538" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G538" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H538" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I538" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J538" t="inlineStr">
+        <is>
+          <t>10:16:58</t>
+        </is>
+      </c>
+      <c r="K538" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>221459</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>محمد الطيب محمد زين</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D539" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E539" t="inlineStr">
+        <is>
+          <t>221459@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F539" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G539" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H539" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I539" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J539" t="inlineStr">
+        <is>
+          <t>10:17:00</t>
+        </is>
+      </c>
+      <c r="K539" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>221536</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>عبده دفع الله سليمان كوكو</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D540" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E540" t="inlineStr">
+        <is>
+          <t>221536@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F540" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G540" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H540" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I540" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J540" t="inlineStr">
+        <is>
+          <t>10:17:18</t>
+        </is>
+      </c>
+      <c r="K540" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>221606</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>راوية الطاهر عبدالله ناصر</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D541" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E541" t="inlineStr">
+        <is>
+          <t>221606@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F541" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G541" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H541" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I541" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J541" t="inlineStr">
+        <is>
+          <t>10:17:25</t>
+        </is>
+      </c>
+      <c r="K541" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>221631</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>رغد الحاج حسين عبدالمتعال</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D542" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E542" t="inlineStr">
+        <is>
+          <t>221631@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F542" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G542" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H542" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I542" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J542" t="inlineStr">
+        <is>
+          <t>10:17:25</t>
+        </is>
+      </c>
+      <c r="K542" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>221569</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>هبه جعفر محمد شوكت</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D543" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E543" t="inlineStr">
+        <is>
+          <t>221569@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F543" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G543" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H543" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I543" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J543" t="inlineStr">
+        <is>
+          <t>10:17:27</t>
+        </is>
+      </c>
+      <c r="K543" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>221756</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>ماريا صالح حسن مثنى محمد</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E544" t="inlineStr">
+        <is>
+          <t>221756@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F544" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G544" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H544" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I544" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J544" t="inlineStr">
+        <is>
+          <t>10:17:29</t>
+        </is>
+      </c>
+      <c r="K544" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>221579</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>لينا مكرم محمد يسن</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D545" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E545" t="inlineStr">
+        <is>
+          <t>221579@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F545" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G545" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H545" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I545" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J545" t="inlineStr">
+        <is>
+          <t>10:17:29</t>
+        </is>
+      </c>
+      <c r="K545" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>221357</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>عبد الله محمد نصر قناوى</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D546" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E546" t="inlineStr">
+        <is>
+          <t>221357@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F546" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G546" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H546" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I546" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J546" t="inlineStr">
+        <is>
+          <t>10:17:48</t>
+        </is>
+      </c>
+      <c r="K546" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>221654</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>محمد اسامه بابكر احمد</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D547" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E547" t="inlineStr">
+        <is>
+          <t>221654@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F547" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G547" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H547" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I547" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J547" t="inlineStr">
+        <is>
+          <t>10:19:35</t>
+        </is>
+      </c>
+      <c r="K547" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>221675</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>ساره بنت سعيد بن عثمان الكناني</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E548" t="inlineStr">
+        <is>
+          <t>221675@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F548" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G548" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H548" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I548" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J548" t="inlineStr">
+        <is>
+          <t>10:19:43</t>
+        </is>
+      </c>
+      <c r="K548" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>221653</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>يزن يحيى سليمان طبش</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E549" t="inlineStr">
+        <is>
+          <t>221653@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F549" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G549" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H549" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I549" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J549" t="inlineStr">
+        <is>
+          <t>10:45:00</t>
+        </is>
+      </c>
+      <c r="K549" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>221589</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>أوينق استيفن أجوك مو</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E550" t="inlineStr">
+        <is>
+          <t>221589@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F550" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G550" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H550" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I550" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J550" t="inlineStr">
+        <is>
+          <t>10:45:27</t>
+        </is>
+      </c>
+      <c r="K550" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K518"/>
+  <autoFilter ref="A1:K550"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Daily attendance processing - 2025-11-17 17:46:43
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Summary'!$A$1:$BF$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$550</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$562</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -8176,11 +8176,11 @@
       </c>
       <c r="G34" s="12" t="inlineStr">
         <is>
-          <t>3.4%</t>
+          <t>6.9%</t>
         </is>
       </c>
       <c r="H34" s="13" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I34" s="13" t="n">
         <v>19</v>
@@ -8192,16 +8192,16 @@
         <v>29</v>
       </c>
       <c r="L34" s="13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M34" s="13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N34" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O34" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P34" s="14" t="n">
         <v>1</v>
@@ -8210,7 +8210,7 @@
         <v>0</v>
       </c>
       <c r="R34" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S34" s="14" t="inlineStr">
         <is>
@@ -26089,18 +26089,18 @@
           <t>221355@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F114" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F114" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G114" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H114" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I114" s="13" t="n">
         <v>19</v>
@@ -26112,16 +26112,16 @@
         <v>29</v>
       </c>
       <c r="L114" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M114" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N114" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O114" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P114" s="14" t="n">
         <v>1</v>
@@ -26130,7 +26130,7 @@
         <v>1</v>
       </c>
       <c r="R114" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S114" s="14" t="inlineStr">
         <is>
@@ -35728,11 +35728,11 @@
       </c>
       <c r="G157" s="12" t="inlineStr">
         <is>
-          <t>3.4%</t>
+          <t>6.9%</t>
         </is>
       </c>
       <c r="H157" s="13" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I157" s="13" t="n">
         <v>19</v>
@@ -35744,16 +35744,16 @@
         <v>29</v>
       </c>
       <c r="L157" s="13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M157" s="13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N157" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O157" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P157" s="14" t="n">
         <v>0</v>
@@ -35762,7 +35762,7 @@
         <v>0</v>
       </c>
       <c r="R157" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S157" s="14" t="inlineStr">
         <is>
@@ -35952,11 +35952,11 @@
       </c>
       <c r="G158" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H158" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I158" s="13" t="n">
         <v>19</v>
@@ -35968,16 +35968,16 @@
         <v>29</v>
       </c>
       <c r="L158" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M158" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N158" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O158" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P158" s="14" t="n">
         <v>0</v>
@@ -35986,7 +35986,7 @@
         <v>1</v>
       </c>
       <c r="R158" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S158" s="14" t="inlineStr">
         <is>
@@ -51401,18 +51401,18 @@
           <t>221982@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F227" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F227" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G227" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H227" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I227" s="13" t="n">
         <v>19</v>
@@ -51424,16 +51424,16 @@
         <v>29</v>
       </c>
       <c r="L227" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M227" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N227" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O227" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P227" s="14" t="n">
         <v>0</v>
@@ -51442,7 +51442,7 @@
         <v>1</v>
       </c>
       <c r="R227" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S227" s="14" t="inlineStr">
         <is>
@@ -53648,11 +53648,11 @@
       </c>
       <c r="G237" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H237" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I237" s="13" t="n">
         <v>19</v>
@@ -53664,16 +53664,16 @@
         <v>29</v>
       </c>
       <c r="L237" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M237" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N237" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O237" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P237" s="14" t="n">
         <v>0</v>
@@ -53682,7 +53682,7 @@
         <v>1</v>
       </c>
       <c r="R237" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S237" s="14" t="inlineStr">
         <is>
@@ -54544,11 +54544,11 @@
       </c>
       <c r="G241" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H241" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I241" s="13" t="n">
         <v>19</v>
@@ -54560,16 +54560,16 @@
         <v>29</v>
       </c>
       <c r="L241" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M241" s="13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N241" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O241" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P241" s="14" t="n">
         <v>1</v>
@@ -54578,7 +54578,7 @@
         <v>0</v>
       </c>
       <c r="R241" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S241" s="14" t="inlineStr">
         <is>
@@ -55216,11 +55216,11 @@
       </c>
       <c r="G244" s="12" t="inlineStr">
         <is>
-          <t>3.4%</t>
+          <t>6.9%</t>
         </is>
       </c>
       <c r="H244" s="13" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I244" s="13" t="n">
         <v>19</v>
@@ -55232,16 +55232,16 @@
         <v>29</v>
       </c>
       <c r="L244" s="13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M244" s="13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N244" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O244" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P244" s="14" t="n">
         <v>0</v>
@@ -55250,7 +55250,7 @@
         <v>1</v>
       </c>
       <c r="R244" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S244" s="14" t="inlineStr">
         <is>
@@ -55657,18 +55657,18 @@
           <t>222063@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F246" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F246" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G246" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H246" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I246" s="13" t="n">
         <v>19</v>
@@ -55680,16 +55680,16 @@
         <v>29</v>
       </c>
       <c r="L246" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M246" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N246" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O246" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P246" s="14" t="n">
         <v>0</v>
@@ -55698,7 +55698,7 @@
         <v>1</v>
       </c>
       <c r="R246" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S246" s="14" t="inlineStr">
         <is>
@@ -56112,11 +56112,11 @@
       </c>
       <c r="G248" s="12" t="inlineStr">
         <is>
-          <t>3.4%</t>
+          <t>6.9%</t>
         </is>
       </c>
       <c r="H248" s="13" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I248" s="13" t="n">
         <v>19</v>
@@ -56128,16 +56128,16 @@
         <v>29</v>
       </c>
       <c r="L248" s="13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M248" s="13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N248" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O248" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P248" s="14" t="n">
         <v>0</v>
@@ -56146,7 +56146,7 @@
         <v>0</v>
       </c>
       <c r="R248" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S248" s="14" t="inlineStr">
         <is>
@@ -56560,11 +56560,11 @@
       </c>
       <c r="G250" s="12" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>3.4%</t>
         </is>
       </c>
       <c r="H250" s="13" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I250" s="13" t="n">
         <v>19</v>
@@ -56576,16 +56576,16 @@
         <v>29</v>
       </c>
       <c r="L250" s="13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M250" s="13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N250" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O250" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P250" s="14" t="n">
         <v>0</v>
@@ -56594,7 +56594,7 @@
         <v>0</v>
       </c>
       <c r="R250" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S250" s="14" t="inlineStr">
         <is>
@@ -57008,11 +57008,11 @@
       </c>
       <c r="G252" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H252" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I252" s="13" t="n">
         <v>19</v>
@@ -57024,16 +57024,16 @@
         <v>29</v>
       </c>
       <c r="L252" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M252" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N252" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O252" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P252" s="14" t="n">
         <v>0</v>
@@ -57042,7 +57042,7 @@
         <v>1</v>
       </c>
       <c r="R252" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S252" s="14" t="inlineStr">
         <is>
@@ -57211,7 +57211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K550"/>
+  <dimension ref="A1:K562"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -88465,8 +88465,692 @@
         </is>
       </c>
     </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>222063</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>محمد مصطفى حامد التوم</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D551" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E551" t="inlineStr">
+        <is>
+          <t>222063@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F551" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G551" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H551" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I551" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J551" t="inlineStr">
+        <is>
+          <t>10:41:13</t>
+        </is>
+      </c>
+      <c r="K551" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>221587</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>ليم عثمان السر الشمباتي</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D552" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E552" t="inlineStr">
+        <is>
+          <t>221587@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F552" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G552" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H552" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I552" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J552" t="inlineStr">
+        <is>
+          <t>10:41:16</t>
+        </is>
+      </c>
+      <c r="K552" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>221355</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>لمى ابكر سعيد جبرين محمد</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E553" t="inlineStr">
+        <is>
+          <t>221355@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F553" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G553" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H553" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I553" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J553" t="inlineStr">
+        <is>
+          <t>10:41:20</t>
+        </is>
+      </c>
+      <c r="K553" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>211569</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>سميره محمد عيسى علي</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D554" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E554" t="inlineStr">
+        <is>
+          <t>211569@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F554" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G554" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H554" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I554" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J554" t="inlineStr">
+        <is>
+          <t>10:41:34</t>
+        </is>
+      </c>
+      <c r="K554" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>222035</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>علا عبد الوهاب خليل محمود</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D555" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E555" t="inlineStr">
+        <is>
+          <t>222035@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F555" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G555" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H555" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I555" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J555" t="inlineStr">
+        <is>
+          <t>10:41:40</t>
+        </is>
+      </c>
+      <c r="K555" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>222113</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>ابرار محمد عبد الله عبد الحميد</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E556" t="inlineStr">
+        <is>
+          <t>222113@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F556" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G556" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H556" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I556" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J556" t="inlineStr">
+        <is>
+          <t>10:41:46</t>
+        </is>
+      </c>
+      <c r="K556" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>222097</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>روان محمد عثمان محمد</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D557" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E557" t="inlineStr">
+        <is>
+          <t>222097@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F557" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G557" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H557" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I557" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J557" t="inlineStr">
+        <is>
+          <t>10:41:51</t>
+        </is>
+      </c>
+      <c r="K557" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>221584</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>عزه بنت محمد بن عوض الصمداني</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E558" t="inlineStr">
+        <is>
+          <t>221584@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F558" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G558" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H558" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I558" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J558" t="inlineStr">
+        <is>
+          <t>10:41:58</t>
+        </is>
+      </c>
+      <c r="K558" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>222076</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>ابرار عبد الماجد عبد العزيز عثمان</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D559" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E559" t="inlineStr">
+        <is>
+          <t>222076@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F559" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G559" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H559" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I559" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J559" t="inlineStr">
+        <is>
+          <t>10:42:11</t>
+        </is>
+      </c>
+      <c r="K559" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>222027</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>خيرية عبد الرازق</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D560" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E560" t="inlineStr">
+        <is>
+          <t>222027@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F560" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G560" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H560" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I560" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J560" t="inlineStr">
+        <is>
+          <t>10:42:24</t>
+        </is>
+      </c>
+      <c r="K560" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>221982</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>امنويل اكوى اقوتو كوت</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D561" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E561" t="inlineStr">
+        <is>
+          <t>221982@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F561" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G561" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H561" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I561" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J561" t="inlineStr">
+        <is>
+          <t>10:42:31</t>
+        </is>
+      </c>
+      <c r="K561" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>222056</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>الغالى ادم عيسى رحيل</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D562" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E562" t="inlineStr">
+        <is>
+          <t>222056@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F562" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G562" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H562" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I562" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J562" t="inlineStr">
+        <is>
+          <t>10:42:41</t>
+        </is>
+      </c>
+      <c r="K562" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K550"/>
+  <autoFilter ref="A1:K562"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Daily attendance processing - 2025-11-17 18:29:23
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Summary'!$A$1:$BF$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$562</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$575</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -11984,11 +11984,11 @@
       </c>
       <c r="G51" s="12" t="inlineStr">
         <is>
-          <t>3.4%</t>
+          <t>6.9%</t>
         </is>
       </c>
       <c r="H51" s="13" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I51" s="13" t="n">
         <v>19</v>
@@ -12000,16 +12000,16 @@
         <v>29</v>
       </c>
       <c r="L51" s="13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M51" s="13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N51" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O51" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P51" s="14" t="n">
         <v>0</v>
@@ -12018,7 +12018,7 @@
         <v>0</v>
       </c>
       <c r="R51" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S51" s="14" t="inlineStr">
         <is>
@@ -12649,18 +12649,18 @@
           <t>212160@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F54" s="23" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F54" s="11" t="inlineStr">
+        <is>
+          <t>High Risk</t>
         </is>
       </c>
       <c r="G54" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H54" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I54" s="13" t="n">
         <v>19</v>
@@ -12672,16 +12672,16 @@
         <v>29</v>
       </c>
       <c r="L54" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M54" s="13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N54" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O54" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P54" s="14" t="n">
         <v>0</v>
@@ -12690,7 +12690,7 @@
         <v>1</v>
       </c>
       <c r="R54" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S54" s="14" t="inlineStr">
         <is>
@@ -14448,11 +14448,11 @@
       </c>
       <c r="G62" s="12" t="inlineStr">
         <is>
-          <t>3.4%</t>
+          <t>6.9%</t>
         </is>
       </c>
       <c r="H62" s="13" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I62" s="13" t="n">
         <v>19</v>
@@ -14464,16 +14464,16 @@
         <v>29</v>
       </c>
       <c r="L62" s="13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M62" s="13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N62" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O62" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P62" s="14" t="n">
         <v>0</v>
@@ -14482,7 +14482,7 @@
         <v>0</v>
       </c>
       <c r="R62" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S62" s="14" t="inlineStr">
         <is>
@@ -14665,18 +14665,18 @@
           <t>212318@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F63" s="11" t="inlineStr">
-        <is>
-          <t>High Risk</t>
+      <c r="F63" s="24" t="inlineStr">
+        <is>
+          <t>Moderate Risk</t>
         </is>
       </c>
       <c r="G63" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H63" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I63" s="13" t="n">
         <v>19</v>
@@ -14688,16 +14688,16 @@
         <v>29</v>
       </c>
       <c r="L63" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M63" s="13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N63" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O63" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P63" s="14" t="n">
         <v>1</v>
@@ -14706,7 +14706,7 @@
         <v>1</v>
       </c>
       <c r="R63" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S63" s="14" t="inlineStr">
         <is>
@@ -14896,11 +14896,11 @@
       </c>
       <c r="G64" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H64" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I64" s="13" t="n">
         <v>19</v>
@@ -14912,16 +14912,16 @@
         <v>29</v>
       </c>
       <c r="L64" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M64" s="13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N64" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O64" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P64" s="14" t="n">
         <v>1</v>
@@ -14930,7 +14930,7 @@
         <v>1</v>
       </c>
       <c r="R64" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S64" s="14" t="inlineStr">
         <is>
@@ -16464,11 +16464,11 @@
       </c>
       <c r="G71" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H71" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I71" s="13" t="n">
         <v>19</v>
@@ -16480,16 +16480,16 @@
         <v>29</v>
       </c>
       <c r="L71" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M71" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N71" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O71" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P71" s="14" t="n">
         <v>0</v>
@@ -16498,7 +16498,7 @@
         <v>1</v>
       </c>
       <c r="R71" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S71" s="14" t="inlineStr">
         <is>
@@ -17360,11 +17360,11 @@
       </c>
       <c r="G75" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H75" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I75" s="13" t="n">
         <v>19</v>
@@ -17376,16 +17376,16 @@
         <v>29</v>
       </c>
       <c r="L75" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M75" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N75" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O75" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P75" s="14" t="n">
         <v>0</v>
@@ -17394,7 +17394,7 @@
         <v>0</v>
       </c>
       <c r="R75" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S75" s="14" t="inlineStr">
         <is>
@@ -17584,11 +17584,11 @@
       </c>
       <c r="G76" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H76" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I76" s="13" t="n">
         <v>19</v>
@@ -17600,16 +17600,16 @@
         <v>29</v>
       </c>
       <c r="L76" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M76" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N76" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O76" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P76" s="14" t="n">
         <v>1</v>
@@ -17618,7 +17618,7 @@
         <v>1</v>
       </c>
       <c r="R76" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S76" s="14" t="inlineStr">
         <is>
@@ -18032,11 +18032,11 @@
       </c>
       <c r="G78" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H78" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I78" s="13" t="n">
         <v>19</v>
@@ -18048,16 +18048,16 @@
         <v>29</v>
       </c>
       <c r="L78" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M78" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N78" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O78" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P78" s="14" t="n">
         <v>0</v>
@@ -18066,7 +18066,7 @@
         <v>1</v>
       </c>
       <c r="R78" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S78" s="14" t="inlineStr">
         <is>
@@ -18697,18 +18697,18 @@
           <t>220618@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F81" s="23" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F81" s="11" t="inlineStr">
+        <is>
+          <t>High Risk</t>
         </is>
       </c>
       <c r="G81" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H81" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I81" s="13" t="n">
         <v>19</v>
@@ -18720,16 +18720,16 @@
         <v>29</v>
       </c>
       <c r="L81" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M81" s="13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N81" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O81" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P81" s="14" t="n">
         <v>1</v>
@@ -18738,7 +18738,7 @@
         <v>0</v>
       </c>
       <c r="R81" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S81" s="14" t="inlineStr">
         <is>
@@ -19152,11 +19152,11 @@
       </c>
       <c r="G83" s="12" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>3.4%</t>
         </is>
       </c>
       <c r="H83" s="13" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I83" s="13" t="n">
         <v>19</v>
@@ -19168,16 +19168,16 @@
         <v>29</v>
       </c>
       <c r="L83" s="13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M83" s="13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N83" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O83" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P83" s="14" t="n">
         <v>0</v>
@@ -19186,7 +19186,7 @@
         <v>0</v>
       </c>
       <c r="R83" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S83" s="14" t="inlineStr">
         <is>
@@ -19376,11 +19376,11 @@
       </c>
       <c r="G84" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H84" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I84" s="13" t="n">
         <v>19</v>
@@ -19392,16 +19392,16 @@
         <v>29</v>
       </c>
       <c r="L84" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M84" s="13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N84" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O84" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P84" s="14" t="n">
         <v>0</v>
@@ -19410,7 +19410,7 @@
         <v>1</v>
       </c>
       <c r="R84" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S84" s="14" t="inlineStr">
         <is>
@@ -39984,11 +39984,11 @@
       </c>
       <c r="G176" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H176" s="13" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I176" s="13" t="n">
         <v>19</v>
@@ -40000,16 +40000,16 @@
         <v>29</v>
       </c>
       <c r="L176" s="13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M176" s="13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N176" s="14" t="n">
         <v>5</v>
       </c>
       <c r="O176" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P176" s="14" t="n">
         <v>1</v>
@@ -40018,7 +40018,7 @@
         <v>1</v>
       </c>
       <c r="R176" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S176" s="14" t="inlineStr">
         <is>
@@ -57211,7 +57211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K562"/>
+  <dimension ref="A1:K575"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -89149,8 +89149,749 @@
         </is>
       </c>
     </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>220766</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>ميار بنت خالد بن محمد الشيخ</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D563" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E563" t="inlineStr">
+        <is>
+          <t>220766@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F563" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G563" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H563" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I563" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J563" t="inlineStr">
+        <is>
+          <t>10:16:02</t>
+        </is>
+      </c>
+      <c r="K563" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>212442</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>رميساء محى الدين الامين الطيب</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D564" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E564" t="inlineStr">
+        <is>
+          <t>212442@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F564" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G564" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H564" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I564" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J564" t="inlineStr">
+        <is>
+          <t>10:16:08</t>
+        </is>
+      </c>
+      <c r="K564" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>220428</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>بسمله محمد عبد الحميد محمد</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E565" t="inlineStr">
+        <is>
+          <t>220428@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F565" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G565" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H565" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I565" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J565" t="inlineStr">
+        <is>
+          <t>10:16:19</t>
+        </is>
+      </c>
+      <c r="K565" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>221682</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>سرين حاج صدوق</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E566" t="inlineStr">
+        <is>
+          <t>221682@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F566" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G566" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H566" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I566" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J566" t="inlineStr">
+        <is>
+          <t>10:16:27</t>
+        </is>
+      </c>
+      <c r="K566" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>212318</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>مازن مصدق يس عبد اللطيف</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D567" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E567" t="inlineStr">
+        <is>
+          <t>212318@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F567" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G567" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H567" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I567" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J567" t="inlineStr">
+        <is>
+          <t>10:16:35</t>
+        </is>
+      </c>
+      <c r="K567" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>220743</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>مصطفى كرم سلامه سليمان</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E568" t="inlineStr">
+        <is>
+          <t>220743@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F568" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G568" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H568" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I568" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J568" t="inlineStr">
+        <is>
+          <t>10:16:43</t>
+        </is>
+      </c>
+      <c r="K568" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>212322</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>مهند حافظ عابدين الفاضل</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E569" t="inlineStr">
+        <is>
+          <t>212322@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F569" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G569" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H569" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I569" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J569" t="inlineStr">
+        <is>
+          <t>10:16:49</t>
+        </is>
+      </c>
+      <c r="K569" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>220304</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>احمد الكامل محمد عبدون عثمان</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D570" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E570" t="inlineStr">
+        <is>
+          <t>220304@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F570" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G570" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H570" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I570" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J570" t="inlineStr">
+        <is>
+          <t>10:16:56</t>
+        </is>
+      </c>
+      <c r="K570" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>212308</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>سحر محمد يوسف محمد</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D571" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E571" t="inlineStr">
+        <is>
+          <t>212308@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F571" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G571" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H571" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I571" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J571" t="inlineStr">
+        <is>
+          <t>10:17:04</t>
+        </is>
+      </c>
+      <c r="K571" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>212125</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>راما محمد الحاج محمد</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D572" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E572" t="inlineStr">
+        <is>
+          <t>212125@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F572" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G572" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H572" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I572" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J572" t="inlineStr">
+        <is>
+          <t>10:17:18</t>
+        </is>
+      </c>
+      <c r="K572" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>220618</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>غيداء مرزوق الرفاعى</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D573" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E573" t="inlineStr">
+        <is>
+          <t>220618@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F573" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G573" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H573" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I573" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J573" t="inlineStr">
+        <is>
+          <t>10:17:30</t>
+        </is>
+      </c>
+      <c r="K573" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>212160</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>المى عماد تركمانى</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E574" t="inlineStr">
+        <is>
+          <t>212160@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F574" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G574" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H574" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I574" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J574" t="inlineStr">
+        <is>
+          <t>10:17:41</t>
+        </is>
+      </c>
+      <c r="K574" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>220314</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>احمد ربيع قطب عبد المطلب بهوت</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E575" t="inlineStr">
+        <is>
+          <t>220314@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F575" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="G575" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H575" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="I575" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="J575" t="inlineStr">
+        <is>
+          <t>10:21:42</t>
+        </is>
+      </c>
+      <c r="K575" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K562"/>
+  <autoFilter ref="A1:K575"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Daily attendance processing - 2025-11-19 13:35:20
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_attendance.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Summary'!$A$1:$BH$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$575</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$K$594</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -9062,7 +9062,7 @@
       </c>
       <c r="G37" s="12" t="inlineStr">
         <is>
-          <t>3.4%</t>
+          <t>6.9%</t>
         </is>
       </c>
       <c r="H37" s="12" t="inlineStr">
@@ -9071,7 +9071,7 @@
         </is>
       </c>
       <c r="I37" s="13" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J37" s="13" t="n">
         <v>18</v>
@@ -9086,10 +9086,10 @@
         <v>29</v>
       </c>
       <c r="N37" s="13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O37" s="13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P37" s="14" t="n">
         <v>5</v>
@@ -9120,10 +9120,10 @@
         <v>2</v>
       </c>
       <c r="X37" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y37" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z37" s="15" t="inlineStr">
         <is>
@@ -16875,14 +16875,14 @@
           <t>212442@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F71" s="11" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F71" s="23" t="inlineStr">
+        <is>
+          <t>High Risk</t>
         </is>
       </c>
       <c r="G71" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H71" s="12" t="inlineStr">
@@ -16891,7 +16891,7 @@
         </is>
       </c>
       <c r="I71" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J71" s="13" t="n">
         <v>18</v>
@@ -16906,10 +16906,10 @@
         <v>29</v>
       </c>
       <c r="N71" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O71" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P71" s="14" t="n">
         <v>5</v>
@@ -16940,10 +16940,10 @@
         <v>2</v>
       </c>
       <c r="X71" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y71" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z71" s="15" t="inlineStr">
         <is>
@@ -17565,14 +17565,14 @@
           <t>212543@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F74" s="11" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F74" s="23" t="inlineStr">
+        <is>
+          <t>High Risk</t>
         </is>
       </c>
       <c r="G74" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H74" s="12" t="inlineStr">
@@ -17581,7 +17581,7 @@
         </is>
       </c>
       <c r="I74" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J74" s="13" t="n">
         <v>18</v>
@@ -17596,10 +17596,10 @@
         <v>29</v>
       </c>
       <c r="N74" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O74" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P74" s="14" t="n">
         <v>5</v>
@@ -17630,10 +17630,10 @@
         <v>2</v>
       </c>
       <c r="X74" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y74" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z74" s="15" t="inlineStr">
         <is>
@@ -17795,14 +17795,14 @@
           <t>220304@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F75" s="11" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F75" s="23" t="inlineStr">
+        <is>
+          <t>High Risk</t>
         </is>
       </c>
       <c r="G75" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H75" s="12" t="inlineStr">
@@ -17811,7 +17811,7 @@
         </is>
       </c>
       <c r="I75" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J75" s="13" t="n">
         <v>18</v>
@@ -17826,10 +17826,10 @@
         <v>29</v>
       </c>
       <c r="N75" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O75" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P75" s="14" t="n">
         <v>5</v>
@@ -17860,10 +17860,10 @@
         <v>2</v>
       </c>
       <c r="X75" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y75" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z75" s="15" t="inlineStr">
         <is>
@@ -21942,7 +21942,7 @@
       </c>
       <c r="G93" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H93" s="12" t="inlineStr">
@@ -21951,7 +21951,7 @@
         </is>
       </c>
       <c r="I93" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J93" s="13" t="n">
         <v>18</v>
@@ -21966,10 +21966,10 @@
         <v>29</v>
       </c>
       <c r="N93" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O93" s="13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P93" s="14" t="n">
         <v>5</v>
@@ -22000,10 +22000,10 @@
         <v>2</v>
       </c>
       <c r="X93" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y93" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z93" s="15" t="inlineStr">
         <is>
@@ -22632,7 +22632,7 @@
       </c>
       <c r="G96" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H96" s="12" t="inlineStr">
@@ -22641,7 +22641,7 @@
         </is>
       </c>
       <c r="I96" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J96" s="13" t="n">
         <v>18</v>
@@ -22656,10 +22656,10 @@
         <v>29</v>
       </c>
       <c r="N96" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O96" s="13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P96" s="14" t="n">
         <v>5</v>
@@ -22690,10 +22690,10 @@
         <v>2</v>
       </c>
       <c r="X96" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y96" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z96" s="15" t="inlineStr">
         <is>
@@ -34362,7 +34362,7 @@
       </c>
       <c r="G147" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H147" s="12" t="inlineStr">
@@ -34371,7 +34371,7 @@
         </is>
       </c>
       <c r="I147" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J147" s="13" t="n">
         <v>18</v>
@@ -34386,10 +34386,10 @@
         <v>29</v>
       </c>
       <c r="N147" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="O147" s="13" t="n">
         <v>5</v>
-      </c>
-      <c r="O147" s="13" t="n">
-        <v>6</v>
       </c>
       <c r="P147" s="14" t="n">
         <v>5</v>
@@ -34420,10 +34420,10 @@
         <v>2</v>
       </c>
       <c r="X147" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y147" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z147" s="15" t="inlineStr">
         <is>
@@ -41952,7 +41952,7 @@
       </c>
       <c r="G180" s="12" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>3.4%</t>
         </is>
       </c>
       <c r="H180" s="12" t="inlineStr">
@@ -41961,7 +41961,7 @@
         </is>
       </c>
       <c r="I180" s="13" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J180" s="13" t="n">
         <v>18</v>
@@ -41976,10 +41976,10 @@
         <v>29</v>
       </c>
       <c r="N180" s="13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O180" s="13" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P180" s="14" t="n">
         <v>5</v>
@@ -42010,10 +42010,10 @@
         <v>2</v>
       </c>
       <c r="X180" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y180" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z180" s="15" t="inlineStr">
         <is>
@@ -42872,7 +42872,7 @@
       </c>
       <c r="G184" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H184" s="12" t="inlineStr">
@@ -42881,7 +42881,7 @@
         </is>
       </c>
       <c r="I184" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J184" s="13" t="n">
         <v>18</v>
@@ -42896,10 +42896,10 @@
         <v>29</v>
       </c>
       <c r="N184" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="O184" s="13" t="n">
         <v>5</v>
-      </c>
-      <c r="O184" s="13" t="n">
-        <v>6</v>
       </c>
       <c r="P184" s="14" t="n">
         <v>5</v>
@@ -42930,10 +42930,10 @@
         <v>2</v>
       </c>
       <c r="X184" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y184" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z184" s="15" t="inlineStr">
         <is>
@@ -45395,14 +45395,14 @@
           <t>221822@med.asu.edu.eg</t>
         </is>
       </c>
-      <c r="F195" s="11" t="inlineStr">
-        <is>
-          <t>Fail</t>
+      <c r="F195" s="23" t="inlineStr">
+        <is>
+          <t>High Risk</t>
         </is>
       </c>
       <c r="G195" s="12" t="inlineStr">
         <is>
-          <t>13.8%</t>
+          <t>17.2%</t>
         </is>
       </c>
       <c r="H195" s="12" t="inlineStr">
@@ -45411,7 +45411,7 @@
         </is>
       </c>
       <c r="I195" s="13" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J195" s="13" t="n">
         <v>18</v>
@@ -45426,10 +45426,10 @@
         <v>29</v>
       </c>
       <c r="N195" s="13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O195" s="13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P195" s="14" t="n">
         <v>5</v>
@@ -45460,10 +45460,10 @@
         <v>2</v>
       </c>
       <c r="X195" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y195" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z195" s="15" t="inlineStr">
         <is>
@@ -45862,7 +45862,7 @@
       </c>
       <c r="G197" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H197" s="12" t="inlineStr">
@@ -45871,7 +45871,7 @@
         </is>
       </c>
       <c r="I197" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J197" s="13" t="n">
         <v>18</v>
@@ -45886,10 +45886,10 @@
         <v>29</v>
       </c>
       <c r="N197" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O197" s="13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P197" s="14" t="n">
         <v>5</v>
@@ -45920,10 +45920,10 @@
         <v>2</v>
       </c>
       <c r="X197" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y197" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z197" s="15" t="inlineStr">
         <is>
@@ -48622,7 +48622,7 @@
       </c>
       <c r="G209" s="12" t="inlineStr">
         <is>
-          <t>10.3%</t>
+          <t>13.8%</t>
         </is>
       </c>
       <c r="H209" s="12" t="inlineStr">
@@ -48631,7 +48631,7 @@
         </is>
       </c>
       <c r="I209" s="13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J209" s="13" t="n">
         <v>18</v>
@@ -48646,10 +48646,10 @@
         <v>29</v>
       </c>
       <c r="N209" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O209" s="13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P209" s="14" t="n">
         <v>5</v>
@@ -48680,10 +48680,10 @@
         <v>2</v>
       </c>
       <c r="X209" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y209" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z209" s="15" t="inlineStr">
         <is>
@@ -51152,7 +51152,7 @@
       </c>
       <c r="G220" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H220" s="12" t="inlineStr">
@@ -51161,7 +51161,7 @@
         </is>
       </c>
       <c r="I220" s="13" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J220" s="13" t="n">
         <v>18</v>
@@ -51176,10 +51176,10 @@
         <v>29</v>
       </c>
       <c r="N220" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O220" s="13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P220" s="14" t="n">
         <v>5</v>
@@ -51210,10 +51210,10 @@
         <v>2</v>
       </c>
       <c r="X220" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y220" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z220" s="15" t="inlineStr">
         <is>
@@ -53912,7 +53912,7 @@
       </c>
       <c r="G232" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H232" s="12" t="inlineStr">
@@ -53921,7 +53921,7 @@
         </is>
       </c>
       <c r="I232" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J232" s="13" t="n">
         <v>18</v>
@@ -53936,10 +53936,10 @@
         <v>29</v>
       </c>
       <c r="N232" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="O232" s="13" t="n">
         <v>5</v>
-      </c>
-      <c r="O232" s="13" t="n">
-        <v>6</v>
       </c>
       <c r="P232" s="14" t="n">
         <v>5</v>
@@ -53970,10 +53970,10 @@
         <v>2</v>
       </c>
       <c r="X232" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y232" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z232" s="15" t="inlineStr">
         <is>
@@ -54142,7 +54142,7 @@
       </c>
       <c r="G233" s="12" t="inlineStr">
         <is>
-          <t>24.1%</t>
+          <t>27.6%</t>
         </is>
       </c>
       <c r="H233" s="12" t="inlineStr">
@@ -54151,7 +54151,7 @@
         </is>
       </c>
       <c r="I233" s="13" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J233" s="13" t="n">
         <v>18</v>
@@ -54166,10 +54166,10 @@
         <v>29</v>
       </c>
       <c r="N233" s="13" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O233" s="13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P233" s="14" t="n">
         <v>5</v>
@@ -54200,10 +54200,10 @@
         <v>2</v>
       </c>
       <c r="X233" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y233" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z233" s="15" t="inlineStr">
         <is>
@@ -55292,7 +55292,7 @@
       </c>
       <c r="G238" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H238" s="12" t="inlineStr">
@@ -55301,7 +55301,7 @@
         </is>
       </c>
       <c r="I238" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J238" s="13" t="n">
         <v>18</v>
@@ -55316,10 +55316,10 @@
         <v>29</v>
       </c>
       <c r="N238" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="O238" s="13" t="n">
         <v>5</v>
-      </c>
-      <c r="O238" s="13" t="n">
-        <v>6</v>
       </c>
       <c r="P238" s="14" t="n">
         <v>5</v>
@@ -55350,10 +55350,10 @@
         <v>2</v>
       </c>
       <c r="X238" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y238" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z238" s="15" t="inlineStr">
         <is>
@@ -56442,7 +56442,7 @@
       </c>
       <c r="G243" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H243" s="12" t="inlineStr">
@@ -56451,7 +56451,7 @@
         </is>
       </c>
       <c r="I243" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J243" s="13" t="n">
         <v>18</v>
@@ -56466,10 +56466,10 @@
         <v>29</v>
       </c>
       <c r="N243" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="O243" s="13" t="n">
         <v>5</v>
-      </c>
-      <c r="O243" s="13" t="n">
-        <v>6</v>
       </c>
       <c r="P243" s="14" t="n">
         <v>5</v>
@@ -56500,10 +56500,10 @@
         <v>2</v>
       </c>
       <c r="X243" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y243" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z243" s="15" t="inlineStr">
         <is>
@@ -56902,7 +56902,7 @@
       </c>
       <c r="G245" s="12" t="inlineStr">
         <is>
-          <t>17.2%</t>
+          <t>20.7%</t>
         </is>
       </c>
       <c r="H245" s="12" t="inlineStr">
@@ -56911,7 +56911,7 @@
         </is>
       </c>
       <c r="I245" s="13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J245" s="13" t="n">
         <v>18</v>
@@ -56926,10 +56926,10 @@
         <v>29</v>
       </c>
       <c r="N245" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="O245" s="13" t="n">
         <v>5</v>
-      </c>
-      <c r="O245" s="13" t="n">
-        <v>6</v>
       </c>
       <c r="P245" s="14" t="n">
         <v>5</v>
@@ -56960,10 +56960,10 @@
         <v>2</v>
       </c>
       <c r="X245" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y245" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z245" s="15" t="inlineStr">
         <is>
@@ -57592,7 +57592,7 @@
       </c>
       <c r="G248" s="12" t="inlineStr">
         <is>
-          <t>6.9%</t>
+          <t>10.3%</t>
         </is>
       </c>
       <c r="H248" s="12" t="inlineStr">
@@ -57601,7 +57601,7 @@
         </is>
       </c>
       <c r="I248" s="13" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J248" s="13" t="n">
         <v>18</v>
@@ -57616,10 +57616,10 @@
         <v>29</v>
       </c>
       <c r="N248" s="13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O248" s="13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P248" s="14" t="n">
         <v>5</v>
@@ -57650,10 +57650,10 @@
         <v>2</v>
       </c>
       <c r="X248" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y248" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z248" s="15" t="inlineStr">
         <is>
@@ -58721,7 +58721,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K575"/>
+  <dimension ref="A1:K594"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -58737,9 +58737,9 @@
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
     <col width="18" customWidth="1" min="11" max="11"/>
@@ -91400,8 +91400,1091 @@
         </is>
       </c>
     </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>221539</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>تحريم شوكات مالك</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E576" t="inlineStr">
+        <is>
+          <t>221539@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F576" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G576" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H576" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I576" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J576" t="inlineStr">
+        <is>
+          <t>11:28:04</t>
+        </is>
+      </c>
+      <c r="K576" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>221755</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>سعدية عاشق</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E577" t="inlineStr">
+        <is>
+          <t>221755@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F577" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G577" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H577" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I577" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J577" t="inlineStr">
+        <is>
+          <t>11:28:16</t>
+        </is>
+      </c>
+      <c r="K577" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>221833</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>صفا محمود صايل صايل</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D578" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E578" t="inlineStr">
+        <is>
+          <t>221833@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F578" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G578" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H578" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I578" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J578" t="inlineStr">
+        <is>
+          <t>11:28:49</t>
+        </is>
+      </c>
+      <c r="K578" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>222058</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>رفا السيد قسم الله السيد</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D579" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E579" t="inlineStr">
+        <is>
+          <t>222058@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F579" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G579" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H579" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I579" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J579" t="inlineStr">
+        <is>
+          <t>11:31:08</t>
+        </is>
+      </c>
+      <c r="K579" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>221904</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>عائشه نور شيهو</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D580" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E580" t="inlineStr">
+        <is>
+          <t>221904@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F580" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G580" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H580" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I580" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J580" t="inlineStr">
+        <is>
+          <t>11:31:54</t>
+        </is>
+      </c>
+      <c r="K580" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>221948</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>سانتينو اتيم شول دينق</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D581" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E581" t="inlineStr">
+        <is>
+          <t>221948@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F581" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G581" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H581" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I581" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J581" t="inlineStr">
+        <is>
+          <t>11:32:33</t>
+        </is>
+      </c>
+      <c r="K581" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>221714</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>زينب عبد اللطيف بيبى فاروق</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D582" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E582" t="inlineStr">
+        <is>
+          <t>221714@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F582" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G582" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H582" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I582" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J582" t="inlineStr">
+        <is>
+          <t>11:34:55</t>
+        </is>
+      </c>
+      <c r="K582" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>221822</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>سعادة يوسف عليو</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D583" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E583" t="inlineStr">
+        <is>
+          <t>221822@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F583" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G583" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H583" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I583" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J583" t="inlineStr">
+        <is>
+          <t>11:35:26</t>
+        </is>
+      </c>
+      <c r="K583" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>211620</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>محمودول اسلام</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D584" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E584" t="inlineStr">
+        <is>
+          <t>211620@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F584" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G584" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H584" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I584" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J584" t="inlineStr">
+        <is>
+          <t>11:35:49</t>
+        </is>
+      </c>
+      <c r="K584" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>222076</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>ابرار عبد الماجد عبد العزيز عثمان</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D585" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E585" t="inlineStr">
+        <is>
+          <t>222076@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F585" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G585" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H585" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I585" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J585" t="inlineStr">
+        <is>
+          <t>11:36:26</t>
+        </is>
+      </c>
+      <c r="K585" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>212442</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>رميساء محى الدين الامين الطيب</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D586" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E586" t="inlineStr">
+        <is>
+          <t>212442@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F586" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G586" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H586" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I586" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J586" t="inlineStr">
+        <is>
+          <t>11:36:42</t>
+        </is>
+      </c>
+      <c r="K586" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>220304</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>احمد الكامل محمد عبدون عثمان</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D587" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E587" t="inlineStr">
+        <is>
+          <t>220304@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F587" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G587" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H587" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I587" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J587" t="inlineStr">
+        <is>
+          <t>11:37:00</t>
+        </is>
+      </c>
+      <c r="K587" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>220967</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>لارا حربي عبدالله الزيادات</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D588" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E588" t="inlineStr">
+        <is>
+          <t>220967@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F588" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G588" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H588" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I588" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J588" t="inlineStr">
+        <is>
+          <t>11:37:18</t>
+        </is>
+      </c>
+      <c r="K588" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>212543</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>زينب سيف الدين محمد ادم</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D589" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E589" t="inlineStr">
+        <is>
+          <t>212543@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F589" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G589" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H589" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I589" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J589" t="inlineStr">
+        <is>
+          <t>11:37:37</t>
+        </is>
+      </c>
+      <c r="K589" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>222028</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>هاجر عبد الحفيظ سيد صالح</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D590" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E590" t="inlineStr">
+        <is>
+          <t>222028@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F590" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G590" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H590" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I590" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J590" t="inlineStr">
+        <is>
+          <t>11:37:49</t>
+        </is>
+      </c>
+      <c r="K590" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>222003</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>اسراء بدر الدين جعفر عثمان</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D591" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E591" t="inlineStr">
+        <is>
+          <t>222003@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F591" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G591" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H591" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I591" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J591" t="inlineStr">
+        <is>
+          <t>11:37:54</t>
+        </is>
+      </c>
+      <c r="K591" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>221000</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>ابوبكر محمد قايد الثوابي</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D592" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E592" t="inlineStr">
+        <is>
+          <t>221000@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F592" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G592" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H592" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I592" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J592" t="inlineStr">
+        <is>
+          <t>11:38:06</t>
+        </is>
+      </c>
+      <c r="K592" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>222004</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>احمد ايمن احمد بشير</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D593" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E593" t="inlineStr">
+        <is>
+          <t>222004@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F593" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G593" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H593" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I593" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J593" t="inlineStr">
+        <is>
+          <t>11:38:18</t>
+        </is>
+      </c>
+      <c r="K593" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>222053</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>صباح سيف الدين عثمان اسحق</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D594" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="E594" t="inlineStr">
+        <is>
+          <t>222053@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="F594" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="G594" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H594" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="I594" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="J594" t="inlineStr">
+        <is>
+          <t>11:38:41</t>
+        </is>
+      </c>
+      <c r="K594" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K575"/>
+  <autoFilter ref="A1:K594"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>